<commit_message>
Created seed project, created Halls, Movies and Screenings seed methods
</commit_message>
<xml_diff>
--- a/LegacyDatabase/EventTypes.xlsx
+++ b/LegacyDatabase/EventTypes.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Cinema\LegacyDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD66E9AD-2C3D-4E1E-8207-30D1927902DE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAFD469-EE36-43E4-8743-597B2F641106}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EventTypes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -369,7 +369,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>